<commit_message>
2 Hour Backup - 1
</commit_message>
<xml_diff>
--- a/Dokumentation_V1.0.0/Zeitplan.xlsx
+++ b/Dokumentation_V1.0.0/Zeitplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moritz\Desktop\Projekte\probst-maveg\Dokumentation_V1.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C0735A-6881-4225-8A92-B9DBAC3729BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24AB9160-ED72-45A7-B748-80F17F315D23}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16260" xr2:uid="{83867029-8E76-3D4F-AE7B-3038CD017D03}"/>
   </bookViews>
@@ -159,9 +159,6 @@
     <t>Merkliste implementieren</t>
   </si>
   <si>
-    <t>Filterfunktion implementieren</t>
-  </si>
-  <si>
     <t>Flexforms erstellen</t>
   </si>
   <si>
@@ -183,13 +180,16 @@
     <t>Activity Diagramme</t>
   </si>
   <si>
-    <t>Datenbank Konzept</t>
-  </si>
-  <si>
     <t>Detailseite implementieren</t>
   </si>
   <si>
     <t>Abgabe / Reserve</t>
+  </si>
+  <si>
+    <t>Filterfunktion + Listview implementieren</t>
+  </si>
+  <si>
+    <t>Datenbankkonzept</t>
   </si>
 </sst>
 </file>
@@ -1005,22 +1005,32 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1053,24 +1063,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1095,24 +1087,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4204,13 +4204,13 @@
       <xdr:col>36</xdr:col>
       <xdr:colOff>85878</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>188686</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
       <xdr:colOff>74774</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>114682</xdr:rowOff>
+      <xdr:rowOff>150968</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4225,7 +4225,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10654092" y="7436757"/>
+          <a:off x="9783235" y="7473043"/>
           <a:ext cx="170325" cy="152782"/>
         </a:xfrm>
         <a:prstGeom prst="diamond">
@@ -4587,7 +4587,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
+      <xdr:colOff>254000</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -4605,7 +4605,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2946400" y="1308100"/>
-          <a:ext cx="3714750" cy="266700"/>
+          <a:ext cx="3911600" cy="266700"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -5006,8 +5006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACB35978-8946-004E-AC9B-C0C1BFAB6460}">
   <dimension ref="A1:CL73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AO28" sqref="AO28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -5213,229 +5213,229 @@
       <c r="CL2" s="18"/>
     </row>
     <row r="3" spans="1:90" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="105"/>
-      <c r="B3" s="108" t="s">
+      <c r="A3" s="109"/>
+      <c r="B3" s="112" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="109"/>
-      <c r="D3" s="110" t="s">
+      <c r="C3" s="113"/>
+      <c r="D3" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="110"/>
-      <c r="F3" s="110"/>
-      <c r="G3" s="109"/>
-      <c r="H3" s="108" t="s">
+      <c r="E3" s="114"/>
+      <c r="F3" s="114"/>
+      <c r="G3" s="113"/>
+      <c r="H3" s="112" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="110"/>
-      <c r="J3" s="110"/>
-      <c r="K3" s="110"/>
-      <c r="L3" s="110"/>
-      <c r="M3" s="110"/>
-      <c r="N3" s="110"/>
-      <c r="O3" s="109"/>
-      <c r="P3" s="108" t="s">
+      <c r="I3" s="114"/>
+      <c r="J3" s="114"/>
+      <c r="K3" s="114"/>
+      <c r="L3" s="114"/>
+      <c r="M3" s="114"/>
+      <c r="N3" s="114"/>
+      <c r="O3" s="113"/>
+      <c r="P3" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" s="110"/>
-      <c r="R3" s="110"/>
-      <c r="S3" s="110"/>
-      <c r="T3" s="110"/>
-      <c r="U3" s="110"/>
-      <c r="V3" s="110"/>
-      <c r="W3" s="109"/>
-      <c r="X3" s="126"/>
-      <c r="Y3" s="108" t="s">
+      <c r="Q3" s="114"/>
+      <c r="R3" s="114"/>
+      <c r="S3" s="114"/>
+      <c r="T3" s="114"/>
+      <c r="U3" s="114"/>
+      <c r="V3" s="114"/>
+      <c r="W3" s="113"/>
+      <c r="X3" s="96"/>
+      <c r="Y3" s="112" t="s">
         <v>27</v>
       </c>
-      <c r="Z3" s="110"/>
-      <c r="AA3" s="110"/>
-      <c r="AB3" s="110"/>
-      <c r="AC3" s="110"/>
-      <c r="AD3" s="110"/>
-      <c r="AE3" s="110"/>
-      <c r="AF3" s="109"/>
-      <c r="AG3" s="110" t="s">
+      <c r="Z3" s="114"/>
+      <c r="AA3" s="114"/>
+      <c r="AB3" s="114"/>
+      <c r="AC3" s="114"/>
+      <c r="AD3" s="114"/>
+      <c r="AE3" s="114"/>
+      <c r="AF3" s="113"/>
+      <c r="AG3" s="114" t="s">
         <v>28</v>
       </c>
-      <c r="AH3" s="110"/>
-      <c r="AI3" s="110"/>
-      <c r="AJ3" s="110"/>
-      <c r="AK3" s="110"/>
-      <c r="AL3" s="110"/>
-      <c r="AM3" s="110"/>
-      <c r="AN3" s="109"/>
-      <c r="AO3" s="108" t="s">
+      <c r="AH3" s="114"/>
+      <c r="AI3" s="114"/>
+      <c r="AJ3" s="114"/>
+      <c r="AK3" s="114"/>
+      <c r="AL3" s="114"/>
+      <c r="AM3" s="114"/>
+      <c r="AN3" s="113"/>
+      <c r="AO3" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="AP3" s="110"/>
-      <c r="AQ3" s="110"/>
-      <c r="AR3" s="110"/>
-      <c r="AS3" s="110"/>
-      <c r="AT3" s="110"/>
-      <c r="AU3" s="110"/>
-      <c r="AV3" s="109"/>
-      <c r="AW3" s="108" t="s">
+      <c r="AP3" s="114"/>
+      <c r="AQ3" s="114"/>
+      <c r="AR3" s="114"/>
+      <c r="AS3" s="114"/>
+      <c r="AT3" s="114"/>
+      <c r="AU3" s="114"/>
+      <c r="AV3" s="113"/>
+      <c r="AW3" s="112" t="s">
         <v>25</v>
       </c>
-      <c r="AX3" s="110"/>
-      <c r="AY3" s="110"/>
-      <c r="AZ3" s="110"/>
-      <c r="BA3" s="110"/>
-      <c r="BB3" s="110"/>
-      <c r="BC3" s="110"/>
-      <c r="BD3" s="109"/>
-      <c r="BE3" s="108" t="s">
+      <c r="AX3" s="114"/>
+      <c r="AY3" s="114"/>
+      <c r="AZ3" s="114"/>
+      <c r="BA3" s="114"/>
+      <c r="BB3" s="114"/>
+      <c r="BC3" s="114"/>
+      <c r="BD3" s="113"/>
+      <c r="BE3" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="BF3" s="110"/>
-      <c r="BG3" s="110"/>
-      <c r="BH3" s="110"/>
-      <c r="BI3" s="110"/>
-      <c r="BJ3" s="110"/>
-      <c r="BK3" s="110"/>
-      <c r="BL3" s="109"/>
+      <c r="BF3" s="114"/>
+      <c r="BG3" s="114"/>
+      <c r="BH3" s="114"/>
+      <c r="BI3" s="114"/>
+      <c r="BJ3" s="114"/>
+      <c r="BK3" s="114"/>
+      <c r="BL3" s="113"/>
       <c r="BM3" s="74"/>
-      <c r="BN3" s="108" t="s">
+      <c r="BN3" s="112" t="s">
         <v>27</v>
       </c>
-      <c r="BO3" s="110"/>
-      <c r="BP3" s="110"/>
-      <c r="BQ3" s="110"/>
-      <c r="BR3" s="110"/>
-      <c r="BS3" s="110"/>
-      <c r="BT3" s="110"/>
-      <c r="BU3" s="110"/>
-      <c r="BV3" s="108" t="s">
+      <c r="BO3" s="114"/>
+      <c r="BP3" s="114"/>
+      <c r="BQ3" s="114"/>
+      <c r="BR3" s="114"/>
+      <c r="BS3" s="114"/>
+      <c r="BT3" s="114"/>
+      <c r="BU3" s="114"/>
+      <c r="BV3" s="112" t="s">
         <v>28</v>
       </c>
-      <c r="BW3" s="110"/>
-      <c r="BX3" s="110"/>
-      <c r="BY3" s="110"/>
-      <c r="BZ3" s="110"/>
-      <c r="CA3" s="110"/>
-      <c r="CB3" s="110"/>
-      <c r="CC3" s="110"/>
-      <c r="CD3" s="108" t="s">
+      <c r="BW3" s="114"/>
+      <c r="BX3" s="114"/>
+      <c r="BY3" s="114"/>
+      <c r="BZ3" s="114"/>
+      <c r="CA3" s="114"/>
+      <c r="CB3" s="114"/>
+      <c r="CC3" s="114"/>
+      <c r="CD3" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="CE3" s="110"/>
-      <c r="CF3" s="110"/>
-      <c r="CG3" s="109"/>
+      <c r="CE3" s="114"/>
+      <c r="CF3" s="114"/>
+      <c r="CG3" s="113"/>
     </row>
     <row r="4" spans="1:90" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="106"/>
-      <c r="B4" s="101" t="s">
+      <c r="A4" s="110"/>
+      <c r="B4" s="105" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="102"/>
-      <c r="D4" s="103">
+      <c r="C4" s="106"/>
+      <c r="D4" s="107">
         <v>44293</v>
       </c>
-      <c r="E4" s="103"/>
-      <c r="F4" s="103"/>
-      <c r="G4" s="104"/>
-      <c r="H4" s="98">
+      <c r="E4" s="107"/>
+      <c r="F4" s="107"/>
+      <c r="G4" s="108"/>
+      <c r="H4" s="123">
         <v>44294</v>
       </c>
-      <c r="I4" s="99"/>
-      <c r="J4" s="99"/>
-      <c r="K4" s="99"/>
-      <c r="L4" s="99"/>
-      <c r="M4" s="99"/>
-      <c r="N4" s="99"/>
-      <c r="O4" s="100"/>
-      <c r="P4" s="98">
+      <c r="I4" s="124"/>
+      <c r="J4" s="124"/>
+      <c r="K4" s="124"/>
+      <c r="L4" s="124"/>
+      <c r="M4" s="124"/>
+      <c r="N4" s="124"/>
+      <c r="O4" s="125"/>
+      <c r="P4" s="123">
         <v>44295</v>
       </c>
-      <c r="Q4" s="99"/>
-      <c r="R4" s="99"/>
-      <c r="S4" s="99"/>
-      <c r="T4" s="99"/>
-      <c r="U4" s="99"/>
-      <c r="V4" s="99"/>
-      <c r="W4" s="100"/>
+      <c r="Q4" s="124"/>
+      <c r="R4" s="124"/>
+      <c r="S4" s="124"/>
+      <c r="T4" s="124"/>
+      <c r="U4" s="124"/>
+      <c r="V4" s="124"/>
+      <c r="W4" s="125"/>
       <c r="X4" s="54"/>
-      <c r="Y4" s="98">
+      <c r="Y4" s="123">
         <v>44298</v>
       </c>
-      <c r="Z4" s="99"/>
-      <c r="AA4" s="99"/>
-      <c r="AB4" s="99"/>
-      <c r="AC4" s="99"/>
-      <c r="AD4" s="99"/>
-      <c r="AE4" s="99"/>
-      <c r="AF4" s="100"/>
-      <c r="AG4" s="98">
+      <c r="Z4" s="124"/>
+      <c r="AA4" s="124"/>
+      <c r="AB4" s="124"/>
+      <c r="AC4" s="124"/>
+      <c r="AD4" s="124"/>
+      <c r="AE4" s="124"/>
+      <c r="AF4" s="125"/>
+      <c r="AG4" s="123">
         <v>44299</v>
       </c>
-      <c r="AH4" s="99"/>
-      <c r="AI4" s="99"/>
-      <c r="AJ4" s="99"/>
-      <c r="AK4" s="99"/>
-      <c r="AL4" s="99"/>
-      <c r="AM4" s="99"/>
-      <c r="AN4" s="100"/>
-      <c r="AO4" s="98">
+      <c r="AH4" s="124"/>
+      <c r="AI4" s="124"/>
+      <c r="AJ4" s="124"/>
+      <c r="AK4" s="124"/>
+      <c r="AL4" s="124"/>
+      <c r="AM4" s="124"/>
+      <c r="AN4" s="125"/>
+      <c r="AO4" s="123">
         <v>44300</v>
       </c>
-      <c r="AP4" s="99"/>
-      <c r="AQ4" s="99"/>
-      <c r="AR4" s="99"/>
-      <c r="AS4" s="99"/>
-      <c r="AT4" s="99"/>
-      <c r="AU4" s="99"/>
-      <c r="AV4" s="100"/>
-      <c r="AW4" s="98">
+      <c r="AP4" s="124"/>
+      <c r="AQ4" s="124"/>
+      <c r="AR4" s="124"/>
+      <c r="AS4" s="124"/>
+      <c r="AT4" s="124"/>
+      <c r="AU4" s="124"/>
+      <c r="AV4" s="125"/>
+      <c r="AW4" s="123">
         <v>44301</v>
       </c>
-      <c r="AX4" s="99"/>
-      <c r="AY4" s="99"/>
-      <c r="AZ4" s="99"/>
-      <c r="BA4" s="99"/>
-      <c r="BB4" s="99"/>
-      <c r="BC4" s="99"/>
-      <c r="BD4" s="100"/>
-      <c r="BE4" s="98">
+      <c r="AX4" s="124"/>
+      <c r="AY4" s="124"/>
+      <c r="AZ4" s="124"/>
+      <c r="BA4" s="124"/>
+      <c r="BB4" s="124"/>
+      <c r="BC4" s="124"/>
+      <c r="BD4" s="125"/>
+      <c r="BE4" s="123">
         <v>44302</v>
       </c>
-      <c r="BF4" s="99"/>
-      <c r="BG4" s="99"/>
-      <c r="BH4" s="99"/>
-      <c r="BI4" s="99"/>
-      <c r="BJ4" s="99"/>
-      <c r="BK4" s="99"/>
-      <c r="BL4" s="100"/>
+      <c r="BF4" s="124"/>
+      <c r="BG4" s="124"/>
+      <c r="BH4" s="124"/>
+      <c r="BI4" s="124"/>
+      <c r="BJ4" s="124"/>
+      <c r="BK4" s="124"/>
+      <c r="BL4" s="125"/>
       <c r="BM4" s="54"/>
-      <c r="BN4" s="98">
+      <c r="BN4" s="123">
         <v>44305</v>
       </c>
-      <c r="BO4" s="99"/>
-      <c r="BP4" s="99"/>
-      <c r="BQ4" s="99"/>
-      <c r="BR4" s="99"/>
-      <c r="BS4" s="99"/>
-      <c r="BT4" s="99"/>
-      <c r="BU4" s="100"/>
-      <c r="BV4" s="98">
+      <c r="BO4" s="124"/>
+      <c r="BP4" s="124"/>
+      <c r="BQ4" s="124"/>
+      <c r="BR4" s="124"/>
+      <c r="BS4" s="124"/>
+      <c r="BT4" s="124"/>
+      <c r="BU4" s="125"/>
+      <c r="BV4" s="123">
         <v>44306</v>
       </c>
-      <c r="BW4" s="99"/>
-      <c r="BX4" s="99"/>
-      <c r="BY4" s="99"/>
-      <c r="BZ4" s="99"/>
-      <c r="CA4" s="99"/>
-      <c r="CB4" s="99"/>
-      <c r="CC4" s="100"/>
-      <c r="CD4" s="98">
+      <c r="BW4" s="124"/>
+      <c r="BX4" s="124"/>
+      <c r="BY4" s="124"/>
+      <c r="BZ4" s="124"/>
+      <c r="CA4" s="124"/>
+      <c r="CB4" s="124"/>
+      <c r="CC4" s="125"/>
+      <c r="CD4" s="123">
         <v>44307</v>
       </c>
-      <c r="CE4" s="99"/>
-      <c r="CF4" s="99"/>
-      <c r="CG4" s="99"/>
+      <c r="CE4" s="124"/>
+      <c r="CF4" s="124"/>
+      <c r="CG4" s="124"/>
     </row>
     <row r="5" spans="1:90" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="107"/>
+      <c r="A5" s="111"/>
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
@@ -5686,15 +5686,15 @@
       </c>
     </row>
     <row r="6" spans="1:90" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="117" t="s">
+      <c r="A6" s="115" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="118"/>
-      <c r="C6" s="118"/>
-      <c r="D6" s="118"/>
-      <c r="E6" s="118"/>
-      <c r="F6" s="118"/>
-      <c r="G6" s="119"/>
+      <c r="B6" s="116"/>
+      <c r="C6" s="116"/>
+      <c r="D6" s="116"/>
+      <c r="E6" s="116"/>
+      <c r="F6" s="116"/>
+      <c r="G6" s="117"/>
       <c r="H6" s="24"/>
       <c r="I6" s="24"/>
       <c r="J6" s="24"/>
@@ -5775,13 +5775,13 @@
       <c r="CG6" s="52"/>
     </row>
     <row r="7" spans="1:90" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="120" t="s">
+      <c r="A7" s="118" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="122">
+      <c r="B7" s="120">
         <v>1</v>
       </c>
-      <c r="C7" s="123">
+      <c r="C7" s="121">
         <v>1</v>
       </c>
       <c r="D7" s="80"/>
@@ -5868,9 +5868,9 @@
       <c r="CG7" s="76"/>
     </row>
     <row r="8" spans="1:90" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="121"/>
-      <c r="B8" s="114"/>
-      <c r="C8" s="124"/>
+      <c r="A8" s="119"/>
+      <c r="B8" s="102"/>
+      <c r="C8" s="122"/>
       <c r="D8" s="93"/>
       <c r="E8" s="63"/>
       <c r="F8" s="6"/>
@@ -5955,13 +5955,13 @@
       <c r="CG8" s="3"/>
     </row>
     <row r="9" spans="1:90" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="111" t="s">
+      <c r="A9" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="113">
+      <c r="B9" s="101">
         <v>2</v>
       </c>
-      <c r="C9" s="115"/>
+      <c r="C9" s="103"/>
       <c r="D9" s="20"/>
       <c r="E9" s="81"/>
       <c r="F9" s="81"/>
@@ -6046,14 +6046,14 @@
       <c r="CG9" s="76"/>
     </row>
     <row r="10" spans="1:90" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="112"/>
-      <c r="B10" s="114"/>
-      <c r="C10" s="116"/>
+      <c r="A10" s="100"/>
+      <c r="B10" s="102"/>
+      <c r="C10" s="104"/>
       <c r="D10" s="6"/>
       <c r="E10" s="93"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
-      <c r="H10" s="125"/>
+      <c r="H10" s="95"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
@@ -6133,13 +6133,13 @@
       <c r="CG10" s="3"/>
     </row>
     <row r="11" spans="1:90" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="111" t="s">
+      <c r="A11" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="113">
+      <c r="B11" s="101">
         <v>2</v>
       </c>
-      <c r="C11" s="115"/>
+      <c r="C11" s="103"/>
       <c r="D11" s="19"/>
       <c r="E11" s="20"/>
       <c r="F11" s="20"/>
@@ -6224,9 +6224,9 @@
       <c r="CG11" s="76"/>
     </row>
     <row r="12" spans="1:90" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="112"/>
-      <c r="B12" s="114"/>
-      <c r="C12" s="116"/>
+      <c r="A12" s="100"/>
+      <c r="B12" s="102"/>
+      <c r="C12" s="104"/>
       <c r="D12" s="2"/>
       <c r="E12" s="6"/>
       <c r="F12" s="93"/>
@@ -6311,20 +6311,20 @@
       <c r="CG12" s="3"/>
     </row>
     <row r="13" spans="1:90" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="111" t="s">
+      <c r="A13" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="113">
+      <c r="B13" s="101">
         <v>2</v>
       </c>
-      <c r="C13" s="115"/>
+      <c r="C13" s="103"/>
       <c r="D13" s="19"/>
       <c r="E13" s="20"/>
       <c r="F13" s="20"/>
       <c r="G13" s="11"/>
       <c r="H13" s="19"/>
       <c r="I13" s="81"/>
-      <c r="J13" s="127"/>
+      <c r="J13" s="97"/>
       <c r="K13" s="20"/>
       <c r="L13" s="20"/>
       <c r="M13" s="20"/>
@@ -6402,9 +6402,9 @@
       <c r="CG13" s="76"/>
     </row>
     <row r="14" spans="1:90" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="112"/>
-      <c r="B14" s="114"/>
-      <c r="C14" s="116"/>
+      <c r="A14" s="100"/>
+      <c r="B14" s="102"/>
+      <c r="C14" s="104"/>
       <c r="D14" s="2"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -6489,13 +6489,13 @@
       <c r="CG14" s="3"/>
     </row>
     <row r="15" spans="1:90" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="111" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="113">
+      <c r="A15" s="99" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="101">
         <v>2</v>
       </c>
-      <c r="C15" s="115"/>
+      <c r="C15" s="103"/>
       <c r="D15" s="20"/>
       <c r="E15" s="20"/>
       <c r="F15" s="20"/>
@@ -6504,7 +6504,7 @@
       <c r="I15" s="20"/>
       <c r="J15" s="64"/>
       <c r="K15" s="81"/>
-      <c r="L15" s="127"/>
+      <c r="L15" s="97"/>
       <c r="M15" s="20"/>
       <c r="N15" s="20"/>
       <c r="O15" s="21"/>
@@ -6580,9 +6580,9 @@
       <c r="CG15" s="76"/>
     </row>
     <row r="16" spans="1:90" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="112"/>
-      <c r="B16" s="114"/>
-      <c r="C16" s="116"/>
+      <c r="A16" s="100"/>
+      <c r="B16" s="102"/>
+      <c r="C16" s="104"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -6595,7 +6595,7 @@
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
       <c r="O16" s="65"/>
-      <c r="P16" s="125"/>
+      <c r="P16" s="95"/>
       <c r="Q16" s="63"/>
       <c r="R16" s="63"/>
       <c r="S16" s="63"/>
@@ -6667,7 +6667,7 @@
       <c r="CG16" s="3"/>
     </row>
     <row r="17" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="129" t="s">
+      <c r="A17" s="128" t="s">
         <v>9</v>
       </c>
       <c r="B17" s="58">
@@ -6684,7 +6684,7 @@
       <c r="K17" s="10"/>
       <c r="L17" s="67"/>
       <c r="M17" s="80"/>
-      <c r="N17" s="127"/>
+      <c r="N17" s="97"/>
       <c r="O17" s="11"/>
       <c r="P17" s="9"/>
       <c r="Q17" s="10"/>
@@ -6758,7 +6758,7 @@
       <c r="CG17" s="76"/>
     </row>
     <row r="18" spans="1:85" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="112"/>
+      <c r="A18" s="100"/>
       <c r="B18" s="47"/>
       <c r="C18" s="48"/>
       <c r="D18" s="6"/>
@@ -6845,8 +6845,8 @@
       <c r="CG18" s="3"/>
     </row>
     <row r="19" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="130" t="s">
-        <v>48</v>
+      <c r="A19" s="126" t="s">
+        <v>47</v>
       </c>
       <c r="B19" s="58">
         <v>1</v>
@@ -6936,7 +6936,7 @@
       <c r="CG19" s="76"/>
     </row>
     <row r="20" spans="1:85" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="131"/>
+      <c r="A20" s="127"/>
       <c r="B20" s="47"/>
       <c r="C20" s="48"/>
       <c r="D20" s="6"/>
@@ -7023,15 +7023,15 @@
       <c r="CG20" s="3"/>
     </row>
     <row r="21" spans="1:85" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="95" t="s">
+      <c r="A21" s="129" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="96"/>
-      <c r="C21" s="96"/>
-      <c r="D21" s="96"/>
-      <c r="E21" s="96"/>
-      <c r="F21" s="96"/>
-      <c r="G21" s="97"/>
+      <c r="B21" s="130"/>
+      <c r="C21" s="130"/>
+      <c r="D21" s="130"/>
+      <c r="E21" s="130"/>
+      <c r="F21" s="130"/>
+      <c r="G21" s="131"/>
       <c r="H21" s="27"/>
       <c r="I21" s="27"/>
       <c r="J21" s="27"/>
@@ -7112,8 +7112,8 @@
       <c r="CG21" s="52"/>
     </row>
     <row r="22" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="129" t="s">
-        <v>49</v>
+      <c r="A22" s="128" t="s">
+        <v>48</v>
       </c>
       <c r="B22" s="58">
         <v>1</v>
@@ -7202,7 +7202,7 @@
       <c r="CG22" s="76"/>
     </row>
     <row r="23" spans="1:85" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="112"/>
+      <c r="A23" s="100"/>
       <c r="B23" s="47"/>
       <c r="C23" s="48"/>
       <c r="D23" s="6"/>
@@ -7289,7 +7289,7 @@
       <c r="CG23" s="3"/>
     </row>
     <row r="24" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="129" t="s">
+      <c r="A24" s="128" t="s">
         <v>10</v>
       </c>
       <c r="B24" s="58">
@@ -7379,7 +7379,7 @@
       <c r="CG24" s="76"/>
     </row>
     <row r="25" spans="1:85" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="112"/>
+      <c r="A25" s="100"/>
       <c r="B25" s="47"/>
       <c r="C25" s="48"/>
       <c r="D25" s="6"/>
@@ -7466,7 +7466,7 @@
       <c r="CG25" s="3"/>
     </row>
     <row r="26" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="129" t="s">
+      <c r="A26" s="128" t="s">
         <v>11</v>
       </c>
       <c r="B26" s="58">
@@ -7556,7 +7556,7 @@
       <c r="CG26" s="76"/>
     </row>
     <row r="27" spans="1:85" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="112"/>
+      <c r="A27" s="100"/>
       <c r="B27" s="47"/>
       <c r="C27" s="48"/>
       <c r="D27" s="6"/>
@@ -7821,7 +7821,7 @@
     </row>
     <row r="30" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="44" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B30" s="58">
         <v>3</v>
@@ -7847,7 +7847,7 @@
       <c r="V30" s="80"/>
       <c r="W30" s="80"/>
       <c r="X30" s="54"/>
-      <c r="Y30" s="127"/>
+      <c r="Y30" s="97"/>
       <c r="Z30" s="10"/>
       <c r="AA30" s="10"/>
       <c r="AB30" s="10"/>
@@ -7934,7 +7934,7 @@
       <c r="V31" s="63"/>
       <c r="W31" s="65"/>
       <c r="X31" s="54"/>
-      <c r="Y31" s="125"/>
+      <c r="Y31" s="95"/>
       <c r="Z31" s="63"/>
       <c r="AA31" s="63"/>
       <c r="AB31" s="6"/>
@@ -8351,7 +8351,7 @@
     </row>
     <row r="36" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="44" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36" s="58">
         <v>2</v>
@@ -9316,7 +9316,7 @@
     </row>
     <row r="47" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="44" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B47" s="58">
         <v>4</v>
@@ -9492,7 +9492,7 @@
     </row>
     <row r="49" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="44" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B49" s="58">
         <v>3</v>
@@ -9720,10 +9720,10 @@
       <c r="AU51" s="67"/>
       <c r="AV51" s="68"/>
       <c r="AW51" s="66"/>
-      <c r="AX51" s="128"/>
-      <c r="AY51" s="128"/>
-      <c r="AZ51" s="128"/>
-      <c r="BA51" s="128"/>
+      <c r="AX51" s="98"/>
+      <c r="AY51" s="98"/>
+      <c r="AZ51" s="98"/>
+      <c r="BA51" s="98"/>
       <c r="BC51" s="10"/>
       <c r="BD51" s="11"/>
       <c r="BE51" s="9"/>
@@ -9845,7 +9845,7 @@
     </row>
     <row r="53" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="44" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B53" s="58">
         <v>4</v>
@@ -9901,10 +9901,10 @@
       <c r="AY53" s="10"/>
       <c r="AZ53" s="10"/>
       <c r="BA53" s="10"/>
-      <c r="BB53" s="128"/>
-      <c r="BC53" s="128"/>
-      <c r="BD53" s="128"/>
-      <c r="BE53" s="128"/>
+      <c r="BB53" s="98"/>
+      <c r="BC53" s="98"/>
+      <c r="BD53" s="98"/>
+      <c r="BE53" s="98"/>
       <c r="BG53" s="10"/>
       <c r="BH53" s="10"/>
       <c r="BI53" s="10"/>
@@ -10022,7 +10022,7 @@
     </row>
     <row r="55" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B55" s="58">
         <v>6</v>
@@ -10800,8 +10800,8 @@
       <c r="BS63" s="10"/>
       <c r="BT63" s="10"/>
       <c r="BU63" s="80"/>
-      <c r="BV63" s="128"/>
-      <c r="BW63" s="128"/>
+      <c r="BV63" s="98"/>
+      <c r="BW63" s="98"/>
       <c r="BY63" s="10"/>
       <c r="BZ63" s="10"/>
       <c r="CA63" s="10"/>
@@ -10901,7 +10901,7 @@
     </row>
     <row r="65" spans="1:85" x14ac:dyDescent="0.35">
       <c r="A65" s="44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B65" s="58">
         <v>2</v>
@@ -11161,7 +11161,7 @@
       <c r="CB67" s="80"/>
       <c r="CC67" s="80"/>
       <c r="CD67" s="80"/>
-      <c r="CE67" s="127"/>
+      <c r="CE67" s="97"/>
       <c r="CF67" s="10"/>
       <c r="CG67" s="77"/>
     </row>
@@ -11254,7 +11254,7 @@
     </row>
     <row r="69" spans="1:85" x14ac:dyDescent="0.35">
       <c r="A69" s="44" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B69" s="49">
         <v>2</v>
@@ -11867,6 +11867,7 @@
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A21:G21"/>
     <mergeCell ref="CD3:CG3"/>
     <mergeCell ref="CD4:CG4"/>
     <mergeCell ref="BV3:CC3"/>
@@ -11879,6 +11880,8 @@
     <mergeCell ref="P4:W4"/>
     <mergeCell ref="Y4:AF4"/>
     <mergeCell ref="AG4:AN4"/>
+    <mergeCell ref="BE4:BL4"/>
+    <mergeCell ref="BN4:BU4"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="C15:C16"/>
@@ -11893,11 +11896,8 @@
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="C13:C14"/>
-    <mergeCell ref="A21:G21"/>
     <mergeCell ref="AO4:AV4"/>
     <mergeCell ref="AW4:BD4"/>
-    <mergeCell ref="BE4:BL4"/>
-    <mergeCell ref="BN4:BU4"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D4:G4"/>
     <mergeCell ref="A3:A5"/>
@@ -11922,7 +11922,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>